<commit_message>
12 cluster sollution for IOP1 clustering
</commit_message>
<xml_diff>
--- a/IOP1_timeline_2/preliminary_tracers_and legend_for lindsay.xlsx
+++ b/IOP1_timeline_2/preliminary_tracers_and legend_for lindsay.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoldsteinGroup\Desktop\Research\GoAmazon_filters\GCxGC_rprojects\New_GCxGC_analysis\IOP1_timeline_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40bfbb23b172f72e/Desktop/R_projects/New_GCxGC_analysis/IOP1_timeline_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CF53CED334D36EB3533AB340FE495DEDAEBE6EE7" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B315CE0C-AF48-41AB-99C8-CB95E9C20838}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12030" windowHeight="6730"/>
+    <workbookView xWindow="1452" yWindow="576" windowWidth="11040" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,20 +428,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="35.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -462,7 +463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -473,7 +474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -484,7 +485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -495,7 +496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -506,27 +507,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>